<commit_message>
Draft of ACS notebook
</commit_message>
<xml_diff>
--- a/census_acs/inputs/acs_variables.xlsx
+++ b/census_acs/inputs/acs_variables.xlsx
@@ -9,11 +9,13 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22095" windowHeight="8835"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22095" windowHeight="8835" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="acs1" sheetId="1" r:id="rId1"/>
     <sheet name="acs2" sheetId="2" r:id="rId2"/>
+    <sheet name="pumas" sheetId="3" r:id="rId3"/>
+    <sheet name="zctas" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1944" uniqueCount="1458">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2216" uniqueCount="1729">
   <si>
     <t>Estimate!!HOUSEHOLDS BY TYPE!!Total households</t>
   </si>
@@ -4399,6 +4401,819 @@
   </si>
   <si>
     <t>Percent Margin of Error!!INCOME AND BENEFITS (IN 2017 INFLATION-ADJUSTED DOLLARS)!!Total households!!Mean household income (dollars)</t>
+  </si>
+  <si>
+    <t>03701</t>
+  </si>
+  <si>
+    <t>03702</t>
+  </si>
+  <si>
+    <t>03703</t>
+  </si>
+  <si>
+    <t>03704</t>
+  </si>
+  <si>
+    <t>03705</t>
+  </si>
+  <si>
+    <t>03706</t>
+  </si>
+  <si>
+    <t>03707</t>
+  </si>
+  <si>
+    <t>03708</t>
+  </si>
+  <si>
+    <t>03709</t>
+  </si>
+  <si>
+    <t>03710</t>
+  </si>
+  <si>
+    <t>03801</t>
+  </si>
+  <si>
+    <t>03802</t>
+  </si>
+  <si>
+    <t>03803</t>
+  </si>
+  <si>
+    <t>03804</t>
+  </si>
+  <si>
+    <t>03805</t>
+  </si>
+  <si>
+    <t>03806</t>
+  </si>
+  <si>
+    <t>03807</t>
+  </si>
+  <si>
+    <t>03808</t>
+  </si>
+  <si>
+    <t>03809</t>
+  </si>
+  <si>
+    <t>03810</t>
+  </si>
+  <si>
+    <t>03901</t>
+  </si>
+  <si>
+    <t>03902</t>
+  </si>
+  <si>
+    <t>03903</t>
+  </si>
+  <si>
+    <t>04001</t>
+  </si>
+  <si>
+    <t>04002</t>
+  </si>
+  <si>
+    <t>04003</t>
+  </si>
+  <si>
+    <t>04004</t>
+  </si>
+  <si>
+    <t>04005</t>
+  </si>
+  <si>
+    <t>04006</t>
+  </si>
+  <si>
+    <t>04007</t>
+  </si>
+  <si>
+    <t>04008</t>
+  </si>
+  <si>
+    <t>04009</t>
+  </si>
+  <si>
+    <t>04010</t>
+  </si>
+  <si>
+    <t>04011</t>
+  </si>
+  <si>
+    <t>04012</t>
+  </si>
+  <si>
+    <t>04013</t>
+  </si>
+  <si>
+    <t>04014</t>
+  </si>
+  <si>
+    <t>04015</t>
+  </si>
+  <si>
+    <t>04016</t>
+  </si>
+  <si>
+    <t>04017</t>
+  </si>
+  <si>
+    <t>04018</t>
+  </si>
+  <si>
+    <t>04101</t>
+  </si>
+  <si>
+    <t>04102</t>
+  </si>
+  <si>
+    <t>04103</t>
+  </si>
+  <si>
+    <t>04104</t>
+  </si>
+  <si>
+    <t>04105</t>
+  </si>
+  <si>
+    <t>04106</t>
+  </si>
+  <si>
+    <t>04107</t>
+  </si>
+  <si>
+    <t>04108</t>
+  </si>
+  <si>
+    <t>04109</t>
+  </si>
+  <si>
+    <t>04110</t>
+  </si>
+  <si>
+    <t>04111</t>
+  </si>
+  <si>
+    <t>04112</t>
+  </si>
+  <si>
+    <t>04113</t>
+  </si>
+  <si>
+    <t>04114</t>
+  </si>
+  <si>
+    <t>10001</t>
+  </si>
+  <si>
+    <t>10002</t>
+  </si>
+  <si>
+    <t>10003</t>
+  </si>
+  <si>
+    <t>10004</t>
+  </si>
+  <si>
+    <t>10005</t>
+  </si>
+  <si>
+    <t>10006</t>
+  </si>
+  <si>
+    <t>10007</t>
+  </si>
+  <si>
+    <t>10009</t>
+  </si>
+  <si>
+    <t>10010</t>
+  </si>
+  <si>
+    <t>10011</t>
+  </si>
+  <si>
+    <t>10012</t>
+  </si>
+  <si>
+    <t>10013</t>
+  </si>
+  <si>
+    <t>10014</t>
+  </si>
+  <si>
+    <t>10016</t>
+  </si>
+  <si>
+    <t>10017</t>
+  </si>
+  <si>
+    <t>10018</t>
+  </si>
+  <si>
+    <t>10019</t>
+  </si>
+  <si>
+    <t>10020</t>
+  </si>
+  <si>
+    <t>10021</t>
+  </si>
+  <si>
+    <t>10022</t>
+  </si>
+  <si>
+    <t>10023</t>
+  </si>
+  <si>
+    <t>10024</t>
+  </si>
+  <si>
+    <t>10025</t>
+  </si>
+  <si>
+    <t>10026</t>
+  </si>
+  <si>
+    <t>10027</t>
+  </si>
+  <si>
+    <t>10028</t>
+  </si>
+  <si>
+    <t>10029</t>
+  </si>
+  <si>
+    <t>10030</t>
+  </si>
+  <si>
+    <t>10031</t>
+  </si>
+  <si>
+    <t>10032</t>
+  </si>
+  <si>
+    <t>10033</t>
+  </si>
+  <si>
+    <t>10034</t>
+  </si>
+  <si>
+    <t>10035</t>
+  </si>
+  <si>
+    <t>10036</t>
+  </si>
+  <si>
+    <t>10037</t>
+  </si>
+  <si>
+    <t>10038</t>
+  </si>
+  <si>
+    <t>10039</t>
+  </si>
+  <si>
+    <t>10040</t>
+  </si>
+  <si>
+    <t>10044</t>
+  </si>
+  <si>
+    <t>10065</t>
+  </si>
+  <si>
+    <t>10069</t>
+  </si>
+  <si>
+    <t>10075</t>
+  </si>
+  <si>
+    <t>10103</t>
+  </si>
+  <si>
+    <t>10110</t>
+  </si>
+  <si>
+    <t>10111</t>
+  </si>
+  <si>
+    <t>10112</t>
+  </si>
+  <si>
+    <t>10115</t>
+  </si>
+  <si>
+    <t>10119</t>
+  </si>
+  <si>
+    <t>10128</t>
+  </si>
+  <si>
+    <t>10152</t>
+  </si>
+  <si>
+    <t>10153</t>
+  </si>
+  <si>
+    <t>10154</t>
+  </si>
+  <si>
+    <t>10162</t>
+  </si>
+  <si>
+    <t>10165</t>
+  </si>
+  <si>
+    <t>10167</t>
+  </si>
+  <si>
+    <t>10168</t>
+  </si>
+  <si>
+    <t>10169</t>
+  </si>
+  <si>
+    <t>10170</t>
+  </si>
+  <si>
+    <t>10171</t>
+  </si>
+  <si>
+    <t>10172</t>
+  </si>
+  <si>
+    <t>10173</t>
+  </si>
+  <si>
+    <t>10174</t>
+  </si>
+  <si>
+    <t>10177</t>
+  </si>
+  <si>
+    <t>10199</t>
+  </si>
+  <si>
+    <t>10271</t>
+  </si>
+  <si>
+    <t>10278</t>
+  </si>
+  <si>
+    <t>10279</t>
+  </si>
+  <si>
+    <t>10280</t>
+  </si>
+  <si>
+    <t>10282</t>
+  </si>
+  <si>
+    <t>10301</t>
+  </si>
+  <si>
+    <t>10302</t>
+  </si>
+  <si>
+    <t>10303</t>
+  </si>
+  <si>
+    <t>10304</t>
+  </si>
+  <si>
+    <t>10305</t>
+  </si>
+  <si>
+    <t>10306</t>
+  </si>
+  <si>
+    <t>10307</t>
+  </si>
+  <si>
+    <t>10308</t>
+  </si>
+  <si>
+    <t>10309</t>
+  </si>
+  <si>
+    <t>10310</t>
+  </si>
+  <si>
+    <t>10311</t>
+  </si>
+  <si>
+    <t>10312</t>
+  </si>
+  <si>
+    <t>10314</t>
+  </si>
+  <si>
+    <t>10451</t>
+  </si>
+  <si>
+    <t>10452</t>
+  </si>
+  <si>
+    <t>10453</t>
+  </si>
+  <si>
+    <t>10454</t>
+  </si>
+  <si>
+    <t>10455</t>
+  </si>
+  <si>
+    <t>10456</t>
+  </si>
+  <si>
+    <t>10457</t>
+  </si>
+  <si>
+    <t>10458</t>
+  </si>
+  <si>
+    <t>10459</t>
+  </si>
+  <si>
+    <t>10460</t>
+  </si>
+  <si>
+    <t>10461</t>
+  </si>
+  <si>
+    <t>10462</t>
+  </si>
+  <si>
+    <t>10463</t>
+  </si>
+  <si>
+    <t>10464</t>
+  </si>
+  <si>
+    <t>10465</t>
+  </si>
+  <si>
+    <t>10466</t>
+  </si>
+  <si>
+    <t>10467</t>
+  </si>
+  <si>
+    <t>10468</t>
+  </si>
+  <si>
+    <t>10469</t>
+  </si>
+  <si>
+    <t>10470</t>
+  </si>
+  <si>
+    <t>10471</t>
+  </si>
+  <si>
+    <t>10472</t>
+  </si>
+  <si>
+    <t>10473</t>
+  </si>
+  <si>
+    <t>10474</t>
+  </si>
+  <si>
+    <t>10475</t>
+  </si>
+  <si>
+    <t>11001</t>
+  </si>
+  <si>
+    <t>11003</t>
+  </si>
+  <si>
+    <t>11004</t>
+  </si>
+  <si>
+    <t>11005</t>
+  </si>
+  <si>
+    <t>11040</t>
+  </si>
+  <si>
+    <t>11101</t>
+  </si>
+  <si>
+    <t>11102</t>
+  </si>
+  <si>
+    <t>11103</t>
+  </si>
+  <si>
+    <t>11104</t>
+  </si>
+  <si>
+    <t>11105</t>
+  </si>
+  <si>
+    <t>11106</t>
+  </si>
+  <si>
+    <t>11109</t>
+  </si>
+  <si>
+    <t>11201</t>
+  </si>
+  <si>
+    <t>11203</t>
+  </si>
+  <si>
+    <t>11204</t>
+  </si>
+  <si>
+    <t>11205</t>
+  </si>
+  <si>
+    <t>11206</t>
+  </si>
+  <si>
+    <t>11207</t>
+  </si>
+  <si>
+    <t>11208</t>
+  </si>
+  <si>
+    <t>11209</t>
+  </si>
+  <si>
+    <t>11210</t>
+  </si>
+  <si>
+    <t>11211</t>
+  </si>
+  <si>
+    <t>11212</t>
+  </si>
+  <si>
+    <t>11213</t>
+  </si>
+  <si>
+    <t>11214</t>
+  </si>
+  <si>
+    <t>11215</t>
+  </si>
+  <si>
+    <t>11216</t>
+  </si>
+  <si>
+    <t>11217</t>
+  </si>
+  <si>
+    <t>11218</t>
+  </si>
+  <si>
+    <t>11219</t>
+  </si>
+  <si>
+    <t>11220</t>
+  </si>
+  <si>
+    <t>11221</t>
+  </si>
+  <si>
+    <t>11222</t>
+  </si>
+  <si>
+    <t>11223</t>
+  </si>
+  <si>
+    <t>11224</t>
+  </si>
+  <si>
+    <t>11225</t>
+  </si>
+  <si>
+    <t>11226</t>
+  </si>
+  <si>
+    <t>11228</t>
+  </si>
+  <si>
+    <t>11229</t>
+  </si>
+  <si>
+    <t>11230</t>
+  </si>
+  <si>
+    <t>11231</t>
+  </si>
+  <si>
+    <t>11232</t>
+  </si>
+  <si>
+    <t>11233</t>
+  </si>
+  <si>
+    <t>11234</t>
+  </si>
+  <si>
+    <t>11235</t>
+  </si>
+  <si>
+    <t>11236</t>
+  </si>
+  <si>
+    <t>11237</t>
+  </si>
+  <si>
+    <t>11238</t>
+  </si>
+  <si>
+    <t>11239</t>
+  </si>
+  <si>
+    <t>11351</t>
+  </si>
+  <si>
+    <t>11354</t>
+  </si>
+  <si>
+    <t>11355</t>
+  </si>
+  <si>
+    <t>11356</t>
+  </si>
+  <si>
+    <t>11357</t>
+  </si>
+  <si>
+    <t>11358</t>
+  </si>
+  <si>
+    <t>11359</t>
+  </si>
+  <si>
+    <t>11360</t>
+  </si>
+  <si>
+    <t>11361</t>
+  </si>
+  <si>
+    <t>11362</t>
+  </si>
+  <si>
+    <t>11363</t>
+  </si>
+  <si>
+    <t>11364</t>
+  </si>
+  <si>
+    <t>11365</t>
+  </si>
+  <si>
+    <t>11366</t>
+  </si>
+  <si>
+    <t>11367</t>
+  </si>
+  <si>
+    <t>11368</t>
+  </si>
+  <si>
+    <t>11369</t>
+  </si>
+  <si>
+    <t>11370</t>
+  </si>
+  <si>
+    <t>11371</t>
+  </si>
+  <si>
+    <t>11372</t>
+  </si>
+  <si>
+    <t>11373</t>
+  </si>
+  <si>
+    <t>11374</t>
+  </si>
+  <si>
+    <t>11375</t>
+  </si>
+  <si>
+    <t>11377</t>
+  </si>
+  <si>
+    <t>11378</t>
+  </si>
+  <si>
+    <t>11379</t>
+  </si>
+  <si>
+    <t>11385</t>
+  </si>
+  <si>
+    <t>11411</t>
+  </si>
+  <si>
+    <t>11412</t>
+  </si>
+  <si>
+    <t>11413</t>
+  </si>
+  <si>
+    <t>11414</t>
+  </si>
+  <si>
+    <t>11415</t>
+  </si>
+  <si>
+    <t>11416</t>
+  </si>
+  <si>
+    <t>11417</t>
+  </si>
+  <si>
+    <t>11418</t>
+  </si>
+  <si>
+    <t>11419</t>
+  </si>
+  <si>
+    <t>11420</t>
+  </si>
+  <si>
+    <t>11421</t>
+  </si>
+  <si>
+    <t>11422</t>
+  </si>
+  <si>
+    <t>11423</t>
+  </si>
+  <si>
+    <t>11424</t>
+  </si>
+  <si>
+    <t>11425</t>
+  </si>
+  <si>
+    <t>11426</t>
+  </si>
+  <si>
+    <t>11427</t>
+  </si>
+  <si>
+    <t>11428</t>
+  </si>
+  <si>
+    <t>11429</t>
+  </si>
+  <si>
+    <t>11430</t>
+  </si>
+  <si>
+    <t>11432</t>
+  </si>
+  <si>
+    <t>11433</t>
+  </si>
+  <si>
+    <t>11434</t>
+  </si>
+  <si>
+    <t>11435</t>
+  </si>
+  <si>
+    <t>11436</t>
+  </si>
+  <si>
+    <t>11451</t>
+  </si>
+  <si>
+    <t>11581</t>
+  </si>
+  <si>
+    <t>11691</t>
+  </si>
+  <si>
+    <t>11692</t>
+  </si>
+  <si>
+    <t>11693</t>
+  </si>
+  <si>
+    <t>11694</t>
+  </si>
+  <si>
+    <t>11697</t>
+  </si>
+  <si>
+    <t>GEO</t>
   </si>
 </sst>
 </file>
@@ -4434,8 +5249,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -4718,9 +5534,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D249"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A238" workbookViewId="0">
-      <selection activeCell="C249" sqref="C249"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -11555,4 +12369,1402 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A56"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="9.140625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>1728</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>1458</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>1459</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>1460</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>1461</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>1462</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>1463</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>1464</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>1465</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>1466</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>1467</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>1468</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>1469</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>1470</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>1471</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
+        <v>1472</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
+        <v>1473</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
+        <v>1474</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
+        <v>1475</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
+        <v>1476</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
+        <v>1477</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="s">
+        <v>1478</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A23" s="1" t="s">
+        <v>1479</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A24" s="1" t="s">
+        <v>1480</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A25" s="1" t="s">
+        <v>1481</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A26" s="1" t="s">
+        <v>1482</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A27" s="1" t="s">
+        <v>1483</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A28" s="1" t="s">
+        <v>1484</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A29" s="1" t="s">
+        <v>1485</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A30" s="1" t="s">
+        <v>1486</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A31" s="1" t="s">
+        <v>1487</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A32" s="1" t="s">
+        <v>1488</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A33" s="1" t="s">
+        <v>1489</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A34" s="1" t="s">
+        <v>1490</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A35" s="1" t="s">
+        <v>1491</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A36" s="1" t="s">
+        <v>1492</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A37" s="1" t="s">
+        <v>1493</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A38" s="1" t="s">
+        <v>1494</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A39" s="1" t="s">
+        <v>1495</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A40" s="1" t="s">
+        <v>1496</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A41" s="1" t="s">
+        <v>1497</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A42" s="1" t="s">
+        <v>1498</v>
+      </c>
+    </row>
+    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A43" s="1" t="s">
+        <v>1499</v>
+      </c>
+    </row>
+    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A44" s="1" t="s">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A45" s="1" t="s">
+        <v>1501</v>
+      </c>
+    </row>
+    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A46" s="1" t="s">
+        <v>1502</v>
+      </c>
+    </row>
+    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A47" s="1" t="s">
+        <v>1503</v>
+      </c>
+    </row>
+    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A48" s="1" t="s">
+        <v>1504</v>
+      </c>
+    </row>
+    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A49" s="1" t="s">
+        <v>1505</v>
+      </c>
+    </row>
+    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A50" s="1" t="s">
+        <v>1506</v>
+      </c>
+    </row>
+    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A51" s="1" t="s">
+        <v>1507</v>
+      </c>
+    </row>
+    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A52" s="1" t="s">
+        <v>1508</v>
+      </c>
+    </row>
+    <row r="53" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A53" s="1" t="s">
+        <v>1509</v>
+      </c>
+    </row>
+    <row r="54" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A54" s="1" t="s">
+        <v>1510</v>
+      </c>
+    </row>
+    <row r="55" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A55" s="1" t="s">
+        <v>1511</v>
+      </c>
+    </row>
+    <row r="56" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A56" s="1" t="s">
+        <v>1512</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" verticalDpi="2" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A216"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="9.140625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>1728</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>1513</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>1514</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>1515</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>1516</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>1517</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>1518</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>1519</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>1520</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>1521</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>1522</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>1523</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>1524</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>1525</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>1526</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
+        <v>1527</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
+        <v>1528</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
+        <v>1529</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
+        <v>1530</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
+        <v>1531</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
+        <v>1532</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="s">
+        <v>1533</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A23" s="1" t="s">
+        <v>1534</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A24" s="1" t="s">
+        <v>1535</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A25" s="1" t="s">
+        <v>1536</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A26" s="1" t="s">
+        <v>1537</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A27" s="1" t="s">
+        <v>1538</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A28" s="1" t="s">
+        <v>1539</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A29" s="1" t="s">
+        <v>1540</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A30" s="1" t="s">
+        <v>1541</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A31" s="1" t="s">
+        <v>1542</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A32" s="1" t="s">
+        <v>1543</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A33" s="1" t="s">
+        <v>1544</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A34" s="1" t="s">
+        <v>1545</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A35" s="1" t="s">
+        <v>1546</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A36" s="1" t="s">
+        <v>1547</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A37" s="1" t="s">
+        <v>1548</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A38" s="1" t="s">
+        <v>1549</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A39" s="1" t="s">
+        <v>1550</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A40" s="1" t="s">
+        <v>1551</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A41" s="1" t="s">
+        <v>1552</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A42" s="1" t="s">
+        <v>1553</v>
+      </c>
+    </row>
+    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A43" s="1" t="s">
+        <v>1554</v>
+      </c>
+    </row>
+    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A44" s="1" t="s">
+        <v>1555</v>
+      </c>
+    </row>
+    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A45" s="1" t="s">
+        <v>1556</v>
+      </c>
+    </row>
+    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A46" s="1" t="s">
+        <v>1557</v>
+      </c>
+    </row>
+    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A47" s="1" t="s">
+        <v>1558</v>
+      </c>
+    </row>
+    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A48" s="1" t="s">
+        <v>1559</v>
+      </c>
+    </row>
+    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A49" s="1" t="s">
+        <v>1560</v>
+      </c>
+    </row>
+    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A50" s="1" t="s">
+        <v>1561</v>
+      </c>
+    </row>
+    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A51" s="1" t="s">
+        <v>1562</v>
+      </c>
+    </row>
+    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A52" s="1" t="s">
+        <v>1563</v>
+      </c>
+    </row>
+    <row r="53" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A53" s="1" t="s">
+        <v>1564</v>
+      </c>
+    </row>
+    <row r="54" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A54" s="1" t="s">
+        <v>1565</v>
+      </c>
+    </row>
+    <row r="55" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A55" s="1" t="s">
+        <v>1566</v>
+      </c>
+    </row>
+    <row r="56" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A56" s="1" t="s">
+        <v>1567</v>
+      </c>
+    </row>
+    <row r="57" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A57" s="1" t="s">
+        <v>1568</v>
+      </c>
+    </row>
+    <row r="58" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A58" s="1" t="s">
+        <v>1569</v>
+      </c>
+    </row>
+    <row r="59" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A59" s="1" t="s">
+        <v>1570</v>
+      </c>
+    </row>
+    <row r="60" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A60" s="1" t="s">
+        <v>1571</v>
+      </c>
+    </row>
+    <row r="61" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A61" s="1" t="s">
+        <v>1572</v>
+      </c>
+    </row>
+    <row r="62" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A62" s="1" t="s">
+        <v>1573</v>
+      </c>
+    </row>
+    <row r="63" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A63" s="1" t="s">
+        <v>1574</v>
+      </c>
+    </row>
+    <row r="64" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A64" s="1" t="s">
+        <v>1575</v>
+      </c>
+    </row>
+    <row r="65" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A65" s="1" t="s">
+        <v>1576</v>
+      </c>
+    </row>
+    <row r="66" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A66" s="1" t="s">
+        <v>1577</v>
+      </c>
+    </row>
+    <row r="67" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A67" s="1" t="s">
+        <v>1578</v>
+      </c>
+    </row>
+    <row r="68" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A68" s="1" t="s">
+        <v>1579</v>
+      </c>
+    </row>
+    <row r="69" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A69" s="1" t="s">
+        <v>1580</v>
+      </c>
+    </row>
+    <row r="70" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A70" s="1" t="s">
+        <v>1581</v>
+      </c>
+    </row>
+    <row r="71" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A71" s="1" t="s">
+        <v>1582</v>
+      </c>
+    </row>
+    <row r="72" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A72" s="1" t="s">
+        <v>1583</v>
+      </c>
+    </row>
+    <row r="73" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A73" s="1" t="s">
+        <v>1584</v>
+      </c>
+    </row>
+    <row r="74" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A74" s="1" t="s">
+        <v>1585</v>
+      </c>
+    </row>
+    <row r="75" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A75" s="1" t="s">
+        <v>1586</v>
+      </c>
+    </row>
+    <row r="76" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A76" s="1" t="s">
+        <v>1587</v>
+      </c>
+    </row>
+    <row r="77" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A77" s="1" t="s">
+        <v>1588</v>
+      </c>
+    </row>
+    <row r="78" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A78" s="1" t="s">
+        <v>1589</v>
+      </c>
+    </row>
+    <row r="79" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A79" s="1" t="s">
+        <v>1590</v>
+      </c>
+    </row>
+    <row r="80" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A80" s="1" t="s">
+        <v>1591</v>
+      </c>
+    </row>
+    <row r="81" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A81" s="1" t="s">
+        <v>1592</v>
+      </c>
+    </row>
+    <row r="82" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A82" s="1" t="s">
+        <v>1593</v>
+      </c>
+    </row>
+    <row r="83" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A83" s="1" t="s">
+        <v>1594</v>
+      </c>
+    </row>
+    <row r="84" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A84" s="1" t="s">
+        <v>1595</v>
+      </c>
+    </row>
+    <row r="85" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A85" s="1" t="s">
+        <v>1596</v>
+      </c>
+    </row>
+    <row r="86" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A86" s="1" t="s">
+        <v>1597</v>
+      </c>
+    </row>
+    <row r="87" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A87" s="1" t="s">
+        <v>1598</v>
+      </c>
+    </row>
+    <row r="88" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A88" s="1" t="s">
+        <v>1599</v>
+      </c>
+    </row>
+    <row r="89" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A89" s="1" t="s">
+        <v>1600</v>
+      </c>
+    </row>
+    <row r="90" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A90" s="1" t="s">
+        <v>1601</v>
+      </c>
+    </row>
+    <row r="91" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A91" s="1" t="s">
+        <v>1602</v>
+      </c>
+    </row>
+    <row r="92" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A92" s="1" t="s">
+        <v>1603</v>
+      </c>
+    </row>
+    <row r="93" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A93" s="1" t="s">
+        <v>1604</v>
+      </c>
+    </row>
+    <row r="94" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A94" s="1" t="s">
+        <v>1605</v>
+      </c>
+    </row>
+    <row r="95" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A95" s="1" t="s">
+        <v>1606</v>
+      </c>
+    </row>
+    <row r="96" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A96" s="1" t="s">
+        <v>1607</v>
+      </c>
+    </row>
+    <row r="97" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A97" s="1" t="s">
+        <v>1608</v>
+      </c>
+    </row>
+    <row r="98" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A98" s="1" t="s">
+        <v>1609</v>
+      </c>
+    </row>
+    <row r="99" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A99" s="1" t="s">
+        <v>1610</v>
+      </c>
+    </row>
+    <row r="100" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A100" s="1" t="s">
+        <v>1611</v>
+      </c>
+    </row>
+    <row r="101" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A101" s="1" t="s">
+        <v>1612</v>
+      </c>
+    </row>
+    <row r="102" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A102" s="1" t="s">
+        <v>1613</v>
+      </c>
+    </row>
+    <row r="103" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A103" s="1" t="s">
+        <v>1614</v>
+      </c>
+    </row>
+    <row r="104" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A104" s="1" t="s">
+        <v>1615</v>
+      </c>
+    </row>
+    <row r="105" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A105" s="1" t="s">
+        <v>1616</v>
+      </c>
+    </row>
+    <row r="106" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A106" s="1" t="s">
+        <v>1617</v>
+      </c>
+    </row>
+    <row r="107" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A107" s="1" t="s">
+        <v>1618</v>
+      </c>
+    </row>
+    <row r="108" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A108" s="1" t="s">
+        <v>1619</v>
+      </c>
+    </row>
+    <row r="109" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A109" s="1" t="s">
+        <v>1620</v>
+      </c>
+    </row>
+    <row r="110" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A110" s="1" t="s">
+        <v>1621</v>
+      </c>
+    </row>
+    <row r="111" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A111" s="1" t="s">
+        <v>1622</v>
+      </c>
+    </row>
+    <row r="112" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A112" s="1" t="s">
+        <v>1623</v>
+      </c>
+    </row>
+    <row r="113" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A113" s="1" t="s">
+        <v>1624</v>
+      </c>
+    </row>
+    <row r="114" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A114" s="1" t="s">
+        <v>1625</v>
+      </c>
+    </row>
+    <row r="115" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A115" s="1" t="s">
+        <v>1626</v>
+      </c>
+    </row>
+    <row r="116" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A116" s="1" t="s">
+        <v>1627</v>
+      </c>
+    </row>
+    <row r="117" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A117" s="1" t="s">
+        <v>1628</v>
+      </c>
+    </row>
+    <row r="118" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A118" s="1" t="s">
+        <v>1629</v>
+      </c>
+    </row>
+    <row r="119" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A119" s="1" t="s">
+        <v>1630</v>
+      </c>
+    </row>
+    <row r="120" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A120" s="1" t="s">
+        <v>1631</v>
+      </c>
+    </row>
+    <row r="121" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A121" s="1" t="s">
+        <v>1632</v>
+      </c>
+    </row>
+    <row r="122" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A122" s="1" t="s">
+        <v>1633</v>
+      </c>
+    </row>
+    <row r="123" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A123" s="1" t="s">
+        <v>1634</v>
+      </c>
+    </row>
+    <row r="124" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A124" s="1" t="s">
+        <v>1635</v>
+      </c>
+    </row>
+    <row r="125" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A125" s="1" t="s">
+        <v>1636</v>
+      </c>
+    </row>
+    <row r="126" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A126" s="1" t="s">
+        <v>1637</v>
+      </c>
+    </row>
+    <row r="127" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A127" s="1" t="s">
+        <v>1638</v>
+      </c>
+    </row>
+    <row r="128" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A128" s="1" t="s">
+        <v>1639</v>
+      </c>
+    </row>
+    <row r="129" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A129" s="1" t="s">
+        <v>1640</v>
+      </c>
+    </row>
+    <row r="130" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A130" s="1" t="s">
+        <v>1641</v>
+      </c>
+    </row>
+    <row r="131" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A131" s="1" t="s">
+        <v>1642</v>
+      </c>
+    </row>
+    <row r="132" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A132" s="1" t="s">
+        <v>1643</v>
+      </c>
+    </row>
+    <row r="133" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A133" s="1" t="s">
+        <v>1644</v>
+      </c>
+    </row>
+    <row r="134" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A134" s="1" t="s">
+        <v>1645</v>
+      </c>
+    </row>
+    <row r="135" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A135" s="1" t="s">
+        <v>1646</v>
+      </c>
+    </row>
+    <row r="136" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A136" s="1" t="s">
+        <v>1647</v>
+      </c>
+    </row>
+    <row r="137" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A137" s="1" t="s">
+        <v>1648</v>
+      </c>
+    </row>
+    <row r="138" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A138" s="1" t="s">
+        <v>1649</v>
+      </c>
+    </row>
+    <row r="139" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A139" s="1" t="s">
+        <v>1650</v>
+      </c>
+    </row>
+    <row r="140" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A140" s="1" t="s">
+        <v>1651</v>
+      </c>
+    </row>
+    <row r="141" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A141" s="1" t="s">
+        <v>1652</v>
+      </c>
+    </row>
+    <row r="142" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A142" s="1" t="s">
+        <v>1653</v>
+      </c>
+    </row>
+    <row r="143" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A143" s="1" t="s">
+        <v>1654</v>
+      </c>
+    </row>
+    <row r="144" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A144" s="1" t="s">
+        <v>1655</v>
+      </c>
+    </row>
+    <row r="145" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A145" s="1" t="s">
+        <v>1656</v>
+      </c>
+    </row>
+    <row r="146" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A146" s="1" t="s">
+        <v>1657</v>
+      </c>
+    </row>
+    <row r="147" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A147" s="1" t="s">
+        <v>1658</v>
+      </c>
+    </row>
+    <row r="148" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A148" s="1" t="s">
+        <v>1659</v>
+      </c>
+    </row>
+    <row r="149" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A149" s="1" t="s">
+        <v>1660</v>
+      </c>
+    </row>
+    <row r="150" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A150" s="1" t="s">
+        <v>1661</v>
+      </c>
+    </row>
+    <row r="151" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A151" s="1" t="s">
+        <v>1662</v>
+      </c>
+    </row>
+    <row r="152" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A152" s="1" t="s">
+        <v>1663</v>
+      </c>
+    </row>
+    <row r="153" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A153" s="1" t="s">
+        <v>1664</v>
+      </c>
+    </row>
+    <row r="154" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A154" s="1" t="s">
+        <v>1665</v>
+      </c>
+    </row>
+    <row r="155" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A155" s="1" t="s">
+        <v>1666</v>
+      </c>
+    </row>
+    <row r="156" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A156" s="1" t="s">
+        <v>1667</v>
+      </c>
+    </row>
+    <row r="157" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A157" s="1" t="s">
+        <v>1668</v>
+      </c>
+    </row>
+    <row r="158" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A158" s="1" t="s">
+        <v>1669</v>
+      </c>
+    </row>
+    <row r="159" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A159" s="1" t="s">
+        <v>1670</v>
+      </c>
+    </row>
+    <row r="160" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A160" s="1" t="s">
+        <v>1671</v>
+      </c>
+    </row>
+    <row r="161" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A161" s="1" t="s">
+        <v>1672</v>
+      </c>
+    </row>
+    <row r="162" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A162" s="1" t="s">
+        <v>1673</v>
+      </c>
+    </row>
+    <row r="163" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A163" s="1" t="s">
+        <v>1674</v>
+      </c>
+    </row>
+    <row r="164" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A164" s="1" t="s">
+        <v>1675</v>
+      </c>
+    </row>
+    <row r="165" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A165" s="1" t="s">
+        <v>1676</v>
+      </c>
+    </row>
+    <row r="166" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A166" s="1" t="s">
+        <v>1677</v>
+      </c>
+    </row>
+    <row r="167" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A167" s="1" t="s">
+        <v>1678</v>
+      </c>
+    </row>
+    <row r="168" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A168" s="1" t="s">
+        <v>1679</v>
+      </c>
+    </row>
+    <row r="169" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A169" s="1" t="s">
+        <v>1680</v>
+      </c>
+    </row>
+    <row r="170" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A170" s="1" t="s">
+        <v>1681</v>
+      </c>
+    </row>
+    <row r="171" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A171" s="1" t="s">
+        <v>1682</v>
+      </c>
+    </row>
+    <row r="172" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A172" s="1" t="s">
+        <v>1683</v>
+      </c>
+    </row>
+    <row r="173" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A173" s="1" t="s">
+        <v>1684</v>
+      </c>
+    </row>
+    <row r="174" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A174" s="1" t="s">
+        <v>1685</v>
+      </c>
+    </row>
+    <row r="175" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A175" s="1" t="s">
+        <v>1686</v>
+      </c>
+    </row>
+    <row r="176" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A176" s="1" t="s">
+        <v>1687</v>
+      </c>
+    </row>
+    <row r="177" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A177" s="1" t="s">
+        <v>1688</v>
+      </c>
+    </row>
+    <row r="178" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A178" s="1" t="s">
+        <v>1689</v>
+      </c>
+    </row>
+    <row r="179" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A179" s="1" t="s">
+        <v>1690</v>
+      </c>
+    </row>
+    <row r="180" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A180" s="1" t="s">
+        <v>1691</v>
+      </c>
+    </row>
+    <row r="181" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A181" s="1" t="s">
+        <v>1692</v>
+      </c>
+    </row>
+    <row r="182" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A182" s="1" t="s">
+        <v>1693</v>
+      </c>
+    </row>
+    <row r="183" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A183" s="1" t="s">
+        <v>1694</v>
+      </c>
+    </row>
+    <row r="184" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A184" s="1" t="s">
+        <v>1695</v>
+      </c>
+    </row>
+    <row r="185" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A185" s="1" t="s">
+        <v>1696</v>
+      </c>
+    </row>
+    <row r="186" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A186" s="1" t="s">
+        <v>1697</v>
+      </c>
+    </row>
+    <row r="187" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A187" s="1" t="s">
+        <v>1698</v>
+      </c>
+    </row>
+    <row r="188" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A188" s="1" t="s">
+        <v>1699</v>
+      </c>
+    </row>
+    <row r="189" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A189" s="1" t="s">
+        <v>1700</v>
+      </c>
+    </row>
+    <row r="190" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A190" s="1" t="s">
+        <v>1701</v>
+      </c>
+    </row>
+    <row r="191" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A191" s="1" t="s">
+        <v>1702</v>
+      </c>
+    </row>
+    <row r="192" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A192" s="1" t="s">
+        <v>1703</v>
+      </c>
+    </row>
+    <row r="193" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A193" s="1" t="s">
+        <v>1704</v>
+      </c>
+    </row>
+    <row r="194" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A194" s="1" t="s">
+        <v>1705</v>
+      </c>
+    </row>
+    <row r="195" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A195" s="1" t="s">
+        <v>1706</v>
+      </c>
+    </row>
+    <row r="196" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A196" s="1" t="s">
+        <v>1707</v>
+      </c>
+    </row>
+    <row r="197" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A197" s="1" t="s">
+        <v>1708</v>
+      </c>
+    </row>
+    <row r="198" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A198" s="1" t="s">
+        <v>1709</v>
+      </c>
+    </row>
+    <row r="199" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A199" s="1" t="s">
+        <v>1710</v>
+      </c>
+    </row>
+    <row r="200" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A200" s="1" t="s">
+        <v>1711</v>
+      </c>
+    </row>
+    <row r="201" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A201" s="1" t="s">
+        <v>1712</v>
+      </c>
+    </row>
+    <row r="202" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A202" s="1" t="s">
+        <v>1713</v>
+      </c>
+    </row>
+    <row r="203" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A203" s="1" t="s">
+        <v>1714</v>
+      </c>
+    </row>
+    <row r="204" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A204" s="1" t="s">
+        <v>1715</v>
+      </c>
+    </row>
+    <row r="205" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A205" s="1" t="s">
+        <v>1716</v>
+      </c>
+    </row>
+    <row r="206" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A206" s="1" t="s">
+        <v>1717</v>
+      </c>
+    </row>
+    <row r="207" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A207" s="1" t="s">
+        <v>1718</v>
+      </c>
+    </row>
+    <row r="208" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A208" s="1" t="s">
+        <v>1719</v>
+      </c>
+    </row>
+    <row r="209" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A209" s="1" t="s">
+        <v>1720</v>
+      </c>
+    </row>
+    <row r="210" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A210" s="1" t="s">
+        <v>1721</v>
+      </c>
+    </row>
+    <row r="211" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A211" s="1" t="s">
+        <v>1722</v>
+      </c>
+    </row>
+    <row r="212" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A212" s="1" t="s">
+        <v>1723</v>
+      </c>
+    </row>
+    <row r="213" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A213" s="1" t="s">
+        <v>1724</v>
+      </c>
+    </row>
+    <row r="214" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A214" s="1" t="s">
+        <v>1725</v>
+      </c>
+    </row>
+    <row r="215" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A215" s="1" t="s">
+        <v>1726</v>
+      </c>
+    </row>
+    <row r="216" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A216" s="1" t="s">
+        <v>1727</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" verticalDpi="2" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>